<commit_message>
up to writing formulae in excel
</commit_message>
<xml_diff>
--- a/spreadsheets/excel/my_workbook.xlsx
+++ b/spreadsheets/excel/my_workbook.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +50,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +413,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -428,7 +428,47 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>lecxE olleH</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Greetings</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Hi Olivia</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>